<commit_message>
Applied AoVI and AAI for VSM of all fault types
</commit_message>
<xml_diff>
--- a/Branch.xlsx
+++ b/Branch.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="47">
   <si>
     <t>From Number</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>C0</t>
+  </si>
+  <si>
+    <t>Distance</t>
   </si>
   <si>
     <t>ANISLAGAN</t>
@@ -159,8 +162,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;₱&quot;* #,##0.00_-;\-&quot;₱&quot;* #,##0.00_-;_-&quot;₱&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;₱&quot;* #,##0_-;\-&quot;₱&quot;* #,##0_-;_-&quot;₱&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;₱&quot;* #,##0.00_-;\-&quot;₱&quot;* #,##0.00_-;_-&quot;₱&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -174,19 +177,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -201,6 +198,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -210,14 +230,13 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -233,54 +252,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -296,6 +269,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -303,15 +283,38 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,31 +329,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,31 +347,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,7 +383,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,73 +479,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,21 +524,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -550,17 +538,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,28 +585,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -622,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -640,130 +643,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1093,10 +1096,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1110,7 +1113,7 @@
     <col min="9" max="11" width="5.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1144,22 +1147,25 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>0.06616</v>
@@ -1179,22 +1185,25 @@
       <c r="K2">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>0.0147</v>
@@ -1214,22 +1223,25 @@
       <c r="K3">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>0.06616</v>
@@ -1249,22 +1261,25 @@
       <c r="K4">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>0.12698</v>
@@ -1284,22 +1299,25 @@
       <c r="K5">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>0.06616</v>
@@ -1319,22 +1337,25 @@
       <c r="K6">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>0.01103</v>
@@ -1354,22 +1375,25 @@
       <c r="K7">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <v>0.01103</v>
@@ -1389,22 +1413,25 @@
       <c r="K8">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9">
         <v>0.07351</v>
@@ -1424,22 +1451,25 @@
       <c r="K9">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F10">
         <v>0.12698</v>
@@ -1459,22 +1489,25 @@
       <c r="K10">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10">
+        <v>68.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11">
         <v>0.08822</v>
@@ -1494,22 +1527,25 @@
       <c r="K11">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12">
         <v>0.08822</v>
@@ -1529,22 +1565,25 @@
       <c r="K12">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F13">
         <v>0.06616</v>
@@ -1564,22 +1603,25 @@
       <c r="K13">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14">
         <v>0.05881</v>
@@ -1599,22 +1641,25 @@
       <c r="K14">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15">
         <v>0.01838</v>
@@ -1634,22 +1679,25 @@
       <c r="K15">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15">
+        <v>55.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F16">
         <v>0.01838</v>
@@ -1669,22 +1717,25 @@
       <c r="K16">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16">
+        <v>55.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F17">
         <v>0.06249</v>
@@ -1704,22 +1755,25 @@
       <c r="K17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F18">
         <v>0.06249</v>
@@ -1739,22 +1793,25 @@
       <c r="K18">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F19">
         <v>0.10292</v>
@@ -1774,22 +1831,25 @@
       <c r="K19">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F20">
         <v>0.09557</v>
@@ -1809,22 +1869,25 @@
       <c r="K20">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F21">
         <v>0.07719</v>
@@ -1844,22 +1907,25 @@
       <c r="K21">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>0.07719</v>
@@ -1879,22 +1945,25 @@
       <c r="K22">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F23">
         <v>0.02205</v>
@@ -1914,22 +1983,25 @@
       <c r="K23">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C24">
         <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F24">
         <v>0.03676</v>
@@ -1949,22 +2021,25 @@
       <c r="K24">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24">
+        <v>65.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C25">
         <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F25">
         <v>0.05514</v>
@@ -1984,22 +2059,25 @@
       <c r="K25">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F26">
         <v>0.00735</v>
@@ -2019,22 +2097,25 @@
       <c r="K26">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>14</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F27">
         <v>0.02573</v>
@@ -2054,22 +2135,25 @@
       <c r="K27">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27">
+        <v>47.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C28">
         <v>12</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -2089,22 +2173,25 @@
       <c r="K28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>13</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C29">
         <v>14</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F29">
         <v>0.04043</v>
@@ -2124,22 +2211,25 @@
       <c r="K29">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29">
+        <v>81.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C30">
         <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F30">
         <v>0.04043</v>
@@ -2159,22 +2249,25 @@
       <c r="K30">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30">
+        <v>87.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C31">
         <v>15</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F31">
         <v>0.04043</v>
@@ -2194,22 +2287,25 @@
       <c r="K31">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31">
+        <v>87.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C32">
         <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F32">
         <v>0.04043</v>
@@ -2229,22 +2325,25 @@
       <c r="K32">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32">
+        <v>39.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>15</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33">
         <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F33">
         <v>0.04043</v>
@@ -2264,22 +2363,25 @@
       <c r="K33">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33">
+        <v>39.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F34">
         <v>0.05881</v>
@@ -2299,22 +2401,25 @@
       <c r="K34">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>28</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2334,22 +2439,25 @@
       <c r="K35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>18</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F36">
         <v>0.06249</v>
@@ -2369,22 +2477,25 @@
       <c r="K36">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36">
+        <v>80.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>17</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C37">
         <v>18</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F37">
         <v>0.06249</v>
@@ -2404,22 +2515,25 @@
       <c r="K37">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37">
+        <v>80.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>18</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C38">
         <v>27</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2439,22 +2553,25 @@
       <c r="K38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C39">
         <v>29</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2474,22 +2591,25 @@
       <c r="K39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>20</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C40">
         <v>21</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F40">
         <v>0.06616</v>
@@ -2509,22 +2629,25 @@
       <c r="K40">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>20</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C41">
         <v>21</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F41">
         <v>0.06616</v>
@@ -2544,22 +2667,25 @@
       <c r="K41">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>30</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C42">
         <v>20</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2579,22 +2705,25 @@
       <c r="K42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>21</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C43">
         <v>22</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F43">
         <v>0.09189</v>
@@ -2614,22 +2743,25 @@
       <c r="K43">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>21</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C44">
         <v>22</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F44">
         <v>0.09189</v>
@@ -2649,22 +2781,25 @@
       <c r="K44">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>21</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C45">
         <v>32</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F45">
         <v>0.05808</v>
@@ -2684,22 +2819,25 @@
       <c r="K45">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>22</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C46">
         <v>23</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F46">
         <v>0.08087</v>
@@ -2719,22 +2857,25 @@
       <c r="K46">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>22</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C47">
         <v>23</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F47">
         <v>0.08087</v>
@@ -2754,22 +2895,25 @@
       <c r="K47">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="L47">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>23</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C48">
         <v>24</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F48">
         <v>0.02463</v>
@@ -2789,22 +2933,25 @@
       <c r="K48">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="L48">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49">
         <v>23</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C49">
         <v>24</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F49">
         <v>0.02463</v>
@@ -2824,22 +2971,25 @@
       <c r="K49">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="L49">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>25</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C50">
         <v>26</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F50">
         <v>0.01523</v>
@@ -2859,22 +3009,25 @@
       <c r="K50">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="L50">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>25</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C51">
         <v>26</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F51">
         <v>0.01523</v>
@@ -2894,22 +3047,25 @@
       <c r="K51">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="L51">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52">
         <v>26</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C52">
         <v>31</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F52">
         <v>0.01552</v>
@@ -2929,22 +3085,25 @@
       <c r="K52">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="L52">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53">
         <v>26</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C53">
         <v>31</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F53">
         <v>0.01552</v>
@@ -2964,22 +3123,25 @@
       <c r="K53">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="L53">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54">
         <v>27</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C54">
         <v>28</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F54">
         <v>0.43562</v>
@@ -2999,22 +3161,25 @@
       <c r="K54">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="L54">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55">
         <v>27</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C55">
         <v>29</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F55">
         <v>0.35875</v>
@@ -3034,22 +3199,25 @@
       <c r="K55">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="L55">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56">
         <v>30</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C56">
         <v>31</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F56">
         <v>0.01724</v>
@@ -3069,22 +3237,25 @@
       <c r="K56">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="L56">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57">
         <v>30</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C57">
         <v>31</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F57">
         <v>0.01724</v>
@@ -3103,6 +3274,9 @@
       </c>
       <c r="K57">
         <v>0.01</v>
+      </c>
+      <c r="L57">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>